<commit_message>
adding rest assured things and some comments in the code :)
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/qaautomation (1).xlsx
+++ b/src/main/java/TestData/qaautomation (1).xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\IdeaProjects\QAAssignment\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9191"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9191" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="197">
   <si>
     <t>Series Cast</t>
   </si>
@@ -177,15 +177,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>{
-    "first_name": "Ali",
-    "last_name": "Ahmad",
-    "email": "ali.ahmad@gmail.com",
-    "password": "12345",
-    "confirm_password": "12345"
-}</t>
   </si>
   <si>
     <t>{
@@ -636,12 +627,25 @@
   </si>
   <si>
     <t>tony.waesymswf@gmail.com</t>
+  </si>
+  <si>
+    <t>{
+    "first_name": "Ali",
+    "last_name": "Ahmad",
+    "email": "ali.ahmad12332@gmail.com",
+    "password": "12345",
+    "confirm_password": "12345"
+}</t>
+  </si>
+  <si>
+    <t>Julian Kane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -768,14 +772,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,23 +1064,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -1108,8 +1112,8 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>59</v>
+      <c r="B5" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1117,7 +1121,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -1183,32 +1187,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.77734375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.109375" style="3" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="3" width="31.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="11.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="14.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="8.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="9.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="13.5546875" collapsed="true"/>
+    <col min="8" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="D1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="109.25" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -1221,7 +1225,7 @@
         <v>48</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>43</v>
@@ -1257,7 +1261,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="105.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="197.25" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>46</v>
       </c>
@@ -1265,10 +1269,10 @@
         <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
@@ -1281,18 +1285,18 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="92.35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="92.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4">
         <v>200</v>
@@ -1305,7 +1309,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1315,7 +1319,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1325,7 +1329,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1335,7 +1339,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1345,7 +1349,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1373,22 +1377,22 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1584,9 +1588,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.2" x14ac:dyDescent="0.35">
@@ -1600,7 +1604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1608,10 +1612,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1619,10 +1623,10 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1630,10 +1634,10 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1641,689 +1645,689 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="13">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="14">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="15">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="16">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="17">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="18">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="19">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>88</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23">
+      <c r="A23" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24">
+      <c r="A24" t="s">
         <v>95</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25">
+      <c r="A25" t="s">
         <v>97</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27">
+      <c r="A27" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28">
+      <c r="A28" t="s">
         <v>103</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29">
+      <c r="A29" t="s">
         <v>105</v>
       </c>
-      <c r="C28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>107</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
         <v>108</v>
-      </c>
-      <c r="B30" t="s">
-        <v>109</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31">
       <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
         <v>110</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32">
       <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" t="s">
         <v>112</v>
-      </c>
-      <c r="B32" t="s">
-        <v>113</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33">
       <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
         <v>114</v>
-      </c>
-      <c r="B33" t="s">
-        <v>115</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34">
       <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
         <v>116</v>
-      </c>
-      <c r="B34" t="s">
-        <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
         <v>118</v>
-      </c>
-      <c r="B35" t="s">
-        <v>119</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="s">
         <v>120</v>
-      </c>
-      <c r="B36" t="s">
-        <v>121</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37">
       <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
         <v>122</v>
-      </c>
-      <c r="B37" t="s">
-        <v>123</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" t="s">
         <v>124</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
         <v>125</v>
       </c>
-      <c r="C38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>126</v>
-      </c>
-      <c r="B39" t="s">
-        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" t="s">
         <v>128</v>
-      </c>
-      <c r="B40" t="s">
-        <v>129</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
         <v>168</v>
       </c>
-      <c r="C41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42">
       <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
         <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>131</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43">
       <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
         <v>132</v>
-      </c>
-      <c r="B43" t="s">
-        <v>133</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
         <v>134</v>
       </c>
-      <c r="B44" t="s">
-        <v>170</v>
-      </c>
-      <c r="C44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>135</v>
-      </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48">
       <c r="A48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
         <v>138</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>185</v>
       </c>
-      <c r="C48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
         <v>139</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>186</v>
-      </c>
-      <c r="C49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>140</v>
-      </c>
-      <c r="B50" t="s">
-        <v>187</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51">
       <c r="A51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
         <v>141</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>188</v>
       </c>
-      <c r="C51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="C52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
         <v>142</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>189</v>
       </c>
-      <c r="C52" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="C53" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
         <v>143</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>190</v>
       </c>
-      <c r="C53" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="C54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
         <v>144</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>191</v>
       </c>
-      <c r="C54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="C55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
         <v>145</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>192</v>
       </c>
-      <c r="C55" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
         <v>146</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>193</v>
       </c>
-      <c r="C56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>147</v>
-      </c>
-      <c r="B57" t="s">
-        <v>194</v>
-      </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" t="s">
         <v>171</v>
       </c>
-      <c r="C58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>162</v>
-      </c>
-      <c r="B59" t="s">
-        <v>172</v>
-      </c>
       <c r="C59" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61">
       <c r="A61" t="s">
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62">
       <c r="A62" t="s">
         <v>13</v>
       </c>
       <c r="B62" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" t="s">
         <v>175</v>
       </c>
-      <c r="C62" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="C63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
         <v>163</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" t="s">
         <v>176</v>
       </c>
-      <c r="C63" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
         <v>164</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>178</v>
       </c>
-      <c r="C64" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="C65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
         <v>165</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>179</v>
       </c>
-      <c r="C65" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="C66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
         <v>166</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>180</v>
       </c>
-      <c r="C66" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>167</v>
-      </c>
-      <c r="B67" t="s">
-        <v>181</v>
-      </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>